<commit_message>
Cambio en Archivo Seguimiento
Se borran los registros de Mario para actualizar
</commit_message>
<xml_diff>
--- a/SEGUIMIENTO_A.xlsx
+++ b/SEGUIMIENTO_A.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gdiazle\Desktop\Respaldo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gdiazle\Documents\GitHub\DocEjecucionBots\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44F28331-E8DB-4593-9A71-0B09BBA29CD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CED911F0-16DB-423D-B98D-D12660D52219}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{4820814D-FDC3-4D82-94A2-679E05A391F6}"/>
+    <workbookView xWindow="1035" yWindow="2145" windowWidth="15375" windowHeight="7875" xr2:uid="{4820814D-FDC3-4D82-94A2-679E05A391F6}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -110,7 +110,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="105">
   <si>
     <t>NO P</t>
   </si>
@@ -923,11 +923,11 @@
   <dimension ref="A1:V55"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="D12" activePane="bottomRight" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
-      <selection pane="bottomRight" activeCell="D16" sqref="D16"/>
+      <selection pane="bottomRight" activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1610,9 +1610,7 @@
       <c r="D14" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="E14" s="1" t="s">
-        <v>64</v>
-      </c>
+      <c r="E14" s="1"/>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
       <c r="H14" t="s">
@@ -1665,9 +1663,7 @@
       <c r="D15" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="E15" s="1" t="s">
-        <v>64</v>
-      </c>
+      <c r="E15" s="1"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
       <c r="H15" t="s">
@@ -1717,9 +1713,7 @@
       <c r="C16" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E16" s="1" t="s">
-        <v>64</v>
-      </c>
+      <c r="E16" s="1"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
       <c r="H16" t="s">
@@ -1769,9 +1763,7 @@
       <c r="C17" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E17" s="1" t="s">
-        <v>64</v>
-      </c>
+      <c r="E17" s="1"/>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
       <c r="H17" t="s">

</xml_diff>